<commit_message>
Arreglado fallo obtencion de boxes, arreglado y cambiado comportamiento texto no validado (ahora aparece todo el texto encontrado aunque la validacion sea de -100), proveedor 70017048 al 100%
</commit_message>
<xml_diff>
--- a/AI_Engine/Resultados/Resultados buenos/dataFrame - 70017048.xlsx
+++ b/AI_Engine/Resultados/Resultados buenos/dataFrame - 70017048.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proyectos\Nueva carpeta\Bot-Creacion-de-Pedidos\AI_Engine\Resultados\Resultados buenos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DBC84E5-AC84-4E9A-9931-A3A1EA8F98AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE261B23-5979-43D3-A460-375DD0CF1731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3900" yWindow="3150" windowWidth="7905" windowHeight="7920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="68">
   <si>
     <t>archivo</t>
   </si>
@@ -139,9 +139,6 @@
     <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\Thyssenkrupp Crankshaft\t132.pdf</t>
   </si>
   <si>
-    <t>500044982</t>
-  </si>
-  <si>
     <t>M 08.2022</t>
   </si>
   <si>
@@ -175,9 +172,6 @@
     <t>C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proveedores\CLIIENTES JOHN DEERE\Thyssenkrupp Crankshaft\t133.pdf</t>
   </si>
   <si>
-    <t>500046156</t>
-  </si>
-  <si>
     <t>M 09.2022</t>
   </si>
   <si>
@@ -245,12 +239,6 @@
   </si>
   <si>
     <t>x</t>
-  </si>
-  <si>
-    <t>Fecha</t>
-  </si>
-  <si>
-    <t>Order number</t>
   </si>
 </sst>
 </file>
@@ -616,22 +604,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:J151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="B119" sqref="B119"/>
+    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.140625" style="2"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" customWidth="1"/>
     <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -686,7 +674,7 @@
         <v>91.986999999999995</v>
       </c>
       <c r="J2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -715,7 +703,7 @@
         <v>90.754000000000005</v>
       </c>
       <c r="J3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -744,7 +732,7 @@
         <v>91.504999999999995</v>
       </c>
       <c r="J4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -773,7 +761,7 @@
         <v>91.986999999999995</v>
       </c>
       <c r="J5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -802,7 +790,7 @@
         <v>91.597999999999999</v>
       </c>
       <c r="J6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -831,7 +819,7 @@
         <v>91.986999999999995</v>
       </c>
       <c r="J7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -860,7 +848,7 @@
         <v>91.986999999999995</v>
       </c>
       <c r="J8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -889,7 +877,7 @@
         <v>91.986999999999995</v>
       </c>
       <c r="J9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -918,7 +906,7 @@
         <v>91.986999999999995</v>
       </c>
       <c r="J10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -947,7 +935,7 @@
         <v>88.254000000000005</v>
       </c>
       <c r="J11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -976,7 +964,7 @@
         <v>88.254000000000005</v>
       </c>
       <c r="J12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1005,10 +993,10 @@
         <v>88.254000000000005</v>
       </c>
       <c r="J13" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1027,11 +1015,14 @@
       <c r="F14" t="s">
         <v>27</v>
       </c>
+      <c r="H14" t="s">
+        <v>54</v>
+      </c>
       <c r="I14">
-        <v>-100</v>
+        <v>88.254000000000005</v>
       </c>
       <c r="J14" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1060,7 +1051,7 @@
         <v>88.254000000000005</v>
       </c>
       <c r="J15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1089,7 +1080,7 @@
         <v>88.254000000000005</v>
       </c>
       <c r="J16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1118,7 +1109,7 @@
         <v>90.554000000000002</v>
       </c>
       <c r="J17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1147,7 +1138,7 @@
         <v>91.504999999999995</v>
       </c>
       <c r="J18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1176,7 +1167,7 @@
         <v>88.492999999999995</v>
       </c>
       <c r="J19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1205,7 +1196,7 @@
         <v>91.986999999999995</v>
       </c>
       <c r="J20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1234,10 +1225,10 @@
         <v>90.658000000000001</v>
       </c>
       <c r="J21" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1256,11 +1247,14 @@
       <c r="F22" t="s">
         <v>19</v>
       </c>
+      <c r="H22" t="s">
+        <v>21</v>
+      </c>
       <c r="I22">
-        <v>-100</v>
+        <v>91.986999999999995</v>
       </c>
       <c r="J22" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1289,7 +1283,7 @@
         <v>91.986999999999995</v>
       </c>
       <c r="J23" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1318,10 +1312,10 @@
         <v>91.986999999999995</v>
       </c>
       <c r="J24" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1329,7 +1323,7 @@
         <v>33</v>
       </c>
       <c r="C25" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D25" t="s">
         <v>10</v>
@@ -1341,16 +1335,16 @@
         <v>14</v>
       </c>
       <c r="H25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I25">
         <v>90.066999999999993</v>
       </c>
       <c r="J25" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1358,7 +1352,7 @@
         <v>33</v>
       </c>
       <c r="C26" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D26" t="s">
         <v>10</v>
@@ -1370,16 +1364,16 @@
         <v>12</v>
       </c>
       <c r="H26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I26">
         <v>90.066999999999993</v>
       </c>
       <c r="J26" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1387,7 +1381,7 @@
         <v>33</v>
       </c>
       <c r="C27" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D27" t="s">
         <v>10</v>
@@ -1399,16 +1393,16 @@
         <v>19</v>
       </c>
       <c r="H27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I27">
         <v>90.066999999999993</v>
       </c>
       <c r="J27" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1416,7 +1410,7 @@
         <v>33</v>
       </c>
       <c r="C28" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D28" t="s">
         <v>10</v>
@@ -1428,16 +1422,16 @@
         <v>12</v>
       </c>
       <c r="H28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I28">
         <v>90.066999999999993</v>
       </c>
       <c r="J28" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1445,7 +1439,7 @@
         <v>33</v>
       </c>
       <c r="C29" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D29" t="s">
         <v>10</v>
@@ -1463,10 +1457,10 @@
         <v>90.066999999999993</v>
       </c>
       <c r="J29" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1474,7 +1468,7 @@
         <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D30" t="s">
         <v>10</v>
@@ -1492,10 +1486,10 @@
         <v>89.902000000000001</v>
       </c>
       <c r="J30" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1503,7 +1497,7 @@
         <v>33</v>
       </c>
       <c r="C31" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D31" t="s">
         <v>10</v>
@@ -1515,16 +1509,16 @@
         <v>12</v>
       </c>
       <c r="H31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I31">
         <v>90.066999999999993</v>
       </c>
       <c r="J31" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1532,7 +1526,7 @@
         <v>33</v>
       </c>
       <c r="C32" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D32" t="s">
         <v>10</v>
@@ -1544,16 +1538,16 @@
         <v>12</v>
       </c>
       <c r="H32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I32">
         <v>90.066999999999993</v>
       </c>
       <c r="J32" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1561,7 +1555,7 @@
         <v>33</v>
       </c>
       <c r="C33" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D33" t="s">
         <v>10</v>
@@ -1573,16 +1567,16 @@
         <v>12</v>
       </c>
       <c r="H33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I33">
         <v>90.066999999999993</v>
       </c>
       <c r="J33" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1590,7 +1584,7 @@
         <v>33</v>
       </c>
       <c r="C34" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D34" t="s">
         <v>10</v>
@@ -1602,16 +1596,16 @@
         <v>12</v>
       </c>
       <c r="H34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I34">
         <v>90.066999999999993</v>
       </c>
       <c r="J34" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1619,7 +1613,7 @@
         <v>33</v>
       </c>
       <c r="C35" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D35" t="s">
         <v>10</v>
@@ -1631,16 +1625,16 @@
         <v>14</v>
       </c>
       <c r="H35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I35">
         <v>90.066999999999993</v>
       </c>
       <c r="J35" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1648,7 +1642,7 @@
         <v>33</v>
       </c>
       <c r="C36" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D36" t="s">
         <v>10</v>
@@ -1666,10 +1660,10 @@
         <v>90.066999999999993</v>
       </c>
       <c r="J36" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1677,7 +1671,7 @@
         <v>33</v>
       </c>
       <c r="C37" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D37" t="s">
         <v>10</v>
@@ -1689,24 +1683,24 @@
         <v>14</v>
       </c>
       <c r="H37" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I37">
         <v>90.066999999999993</v>
       </c>
       <c r="J37" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C38" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D38" t="s">
         <v>10</v>
@@ -1718,53 +1712,53 @@
         <v>27</v>
       </c>
       <c r="H38" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I38">
-        <v>90.043000000000006</v>
+        <v>91.15</v>
       </c>
       <c r="J38" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C39" t="s">
+        <v>25</v>
+      </c>
+      <c r="D39" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" t="s">
+        <v>26</v>
+      </c>
+      <c r="F39" t="s">
         <v>46</v>
       </c>
-      <c r="D39" t="s">
-        <v>10</v>
-      </c>
-      <c r="E39" t="s">
-        <v>26</v>
-      </c>
-      <c r="F39" t="s">
-        <v>48</v>
-      </c>
       <c r="H39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I39">
-        <v>90.043000000000006</v>
+        <v>91.15</v>
       </c>
       <c r="J39" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C40" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D40" t="s">
         <v>10</v>
@@ -1776,24 +1770,24 @@
         <v>28</v>
       </c>
       <c r="H40" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I40">
-        <v>90.043000000000006</v>
+        <v>91.15</v>
       </c>
       <c r="J40" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C41" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D41" t="s">
         <v>10</v>
@@ -1802,27 +1796,27 @@
         <v>26</v>
       </c>
       <c r="F41" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H41" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I41">
-        <v>90.043000000000006</v>
+        <v>91.15</v>
       </c>
       <c r="J41" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C42" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D42" t="s">
         <v>10</v>
@@ -1831,27 +1825,27 @@
         <v>26</v>
       </c>
       <c r="F42" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I42">
-        <v>90.043000000000006</v>
+        <v>91.15</v>
       </c>
       <c r="J42" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C43" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D43" t="s">
         <v>10</v>
@@ -1860,27 +1854,27 @@
         <v>26</v>
       </c>
       <c r="F43" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H43" t="s">
         <v>13</v>
       </c>
       <c r="I43">
-        <v>90.043000000000006</v>
+        <v>91.15</v>
       </c>
       <c r="J43" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C44" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D44" t="s">
         <v>10</v>
@@ -1892,24 +1886,24 @@
         <v>27</v>
       </c>
       <c r="H44" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I44">
-        <v>90.043000000000006</v>
+        <v>91.15</v>
       </c>
       <c r="J44" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C45" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D45" t="s">
         <v>10</v>
@@ -1927,18 +1921,18 @@
         <v>89.902000000000001</v>
       </c>
       <c r="J45" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C46" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D46" t="s">
         <v>10</v>
@@ -1947,27 +1941,27 @@
         <v>26</v>
       </c>
       <c r="F46" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H46" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I46">
-        <v>90.043000000000006</v>
+        <v>91.15</v>
       </c>
       <c r="J46" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C47" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D47" t="s">
         <v>10</v>
@@ -1979,24 +1973,24 @@
         <v>28</v>
       </c>
       <c r="H47" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I47">
-        <v>90.043000000000006</v>
+        <v>91.15</v>
       </c>
       <c r="J47" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C48" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D48" t="s">
         <v>10</v>
@@ -2008,24 +2002,24 @@
         <v>27</v>
       </c>
       <c r="H48" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I48">
-        <v>90.043000000000006</v>
+        <v>91.15</v>
       </c>
       <c r="J48" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C49" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D49" t="s">
         <v>10</v>
@@ -2034,27 +2028,27 @@
         <v>26</v>
       </c>
       <c r="F49" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H49" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I49">
-        <v>90.043000000000006</v>
+        <v>91.15</v>
       </c>
       <c r="J49" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C50" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D50" t="s">
         <v>10</v>
@@ -2066,24 +2060,24 @@
         <v>28</v>
       </c>
       <c r="H50" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I50">
-        <v>90.043000000000006</v>
+        <v>91.15</v>
       </c>
       <c r="J50" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C51" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D51" t="s">
         <v>10</v>
@@ -2092,27 +2086,27 @@
         <v>26</v>
       </c>
       <c r="F51" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H51" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I51">
-        <v>90.043000000000006</v>
+        <v>91.15</v>
       </c>
       <c r="J51" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C52" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D52" t="s">
         <v>10</v>
@@ -2121,27 +2115,27 @@
         <v>26</v>
       </c>
       <c r="F52" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H52" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I52">
-        <v>90.043000000000006</v>
+        <v>91.15</v>
       </c>
       <c r="J52" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C53" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D53" t="s">
         <v>10</v>
@@ -2150,56 +2144,56 @@
         <v>26</v>
       </c>
       <c r="F53" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H53" t="s">
         <v>13</v>
       </c>
       <c r="I53">
-        <v>90.043000000000006</v>
+        <v>91.15</v>
       </c>
       <c r="J53" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C54" t="s">
+        <v>25</v>
+      </c>
+      <c r="D54" t="s">
+        <v>10</v>
+      </c>
+      <c r="E54" t="s">
+        <v>26</v>
+      </c>
+      <c r="F54" t="s">
         <v>46</v>
-      </c>
-      <c r="D54" t="s">
-        <v>10</v>
-      </c>
-      <c r="E54" t="s">
-        <v>26</v>
-      </c>
-      <c r="F54" t="s">
-        <v>48</v>
       </c>
       <c r="H54" t="s">
         <v>15</v>
       </c>
       <c r="I54">
-        <v>90.043000000000006</v>
+        <v>91.15</v>
       </c>
       <c r="J54" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C55" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D55" t="s">
         <v>10</v>
@@ -2211,24 +2205,24 @@
         <v>27</v>
       </c>
       <c r="H55" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I55">
-        <v>90.043000000000006</v>
+        <v>91.15</v>
       </c>
       <c r="J55" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C56" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D56" t="s">
         <v>10</v>
@@ -2243,21 +2237,21 @@
         <v>16</v>
       </c>
       <c r="I56">
-        <v>90.043000000000006</v>
+        <v>91.15</v>
       </c>
       <c r="J56" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C57" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D57" t="s">
         <v>10</v>
@@ -2266,27 +2260,27 @@
         <v>26</v>
       </c>
       <c r="F57" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H57" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I57">
-        <v>90.043000000000006</v>
+        <v>91.15</v>
       </c>
       <c r="J57" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C58" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D58" t="s">
         <v>10</v>
@@ -2298,24 +2292,24 @@
         <v>27</v>
       </c>
       <c r="H58" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I58">
-        <v>90.043000000000006</v>
+        <v>91.15</v>
       </c>
       <c r="J58" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C59" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D59" t="s">
         <v>10</v>
@@ -2330,21 +2324,21 @@
         <v>20</v>
       </c>
       <c r="I59">
-        <v>90.043000000000006</v>
+        <v>91.15</v>
       </c>
       <c r="J59" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C60" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D60" t="s">
         <v>10</v>
@@ -2356,24 +2350,24 @@
         <v>27</v>
       </c>
       <c r="H60" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I60">
-        <v>90.043000000000006</v>
+        <v>91.15</v>
       </c>
       <c r="J60" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C61" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D61" t="s">
         <v>10</v>
@@ -2382,27 +2376,27 @@
         <v>26</v>
       </c>
       <c r="F61" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H61" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I61">
-        <v>90.043000000000006</v>
+        <v>91.15</v>
       </c>
       <c r="J61" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C62" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D62" t="s">
         <v>10</v>
@@ -2414,24 +2408,24 @@
         <v>14</v>
       </c>
       <c r="H62" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I62">
         <v>90.066999999999993</v>
       </c>
       <c r="J62" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C63" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D63" t="s">
         <v>10</v>
@@ -2443,24 +2437,24 @@
         <v>12</v>
       </c>
       <c r="H63" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I63">
         <v>90.066999999999993</v>
       </c>
       <c r="J63" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C64" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D64" t="s">
         <v>10</v>
@@ -2472,24 +2466,24 @@
         <v>14</v>
       </c>
       <c r="H64" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I64">
         <v>90.066999999999993</v>
       </c>
       <c r="J64" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C65" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D65" t="s">
         <v>10</v>
@@ -2501,24 +2495,24 @@
         <v>12</v>
       </c>
       <c r="H65" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I65">
         <v>90.066999999999993</v>
       </c>
       <c r="J65" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C66" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D66" t="s">
         <v>10</v>
@@ -2536,18 +2530,18 @@
         <v>90.066999999999993</v>
       </c>
       <c r="J66" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C67" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D67" t="s">
         <v>10</v>
@@ -2565,18 +2559,18 @@
         <v>90.066999999999993</v>
       </c>
       <c r="J67" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C68" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D68" t="s">
         <v>10</v>
@@ -2594,18 +2588,18 @@
         <v>88.293999999999997</v>
       </c>
       <c r="J68" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C69" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D69" t="s">
         <v>10</v>
@@ -2617,24 +2611,24 @@
         <v>12</v>
       </c>
       <c r="H69" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I69">
         <v>90.066999999999993</v>
       </c>
       <c r="J69" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C70" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D70" t="s">
         <v>10</v>
@@ -2646,24 +2640,24 @@
         <v>12</v>
       </c>
       <c r="H70" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I70">
         <v>90.066999999999993</v>
       </c>
       <c r="J70" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C71" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D71" t="s">
         <v>10</v>
@@ -2675,24 +2669,24 @@
         <v>12</v>
       </c>
       <c r="H71" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I71">
         <v>90.066999999999993</v>
       </c>
       <c r="J71" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>70</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C72" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D72" t="s">
         <v>10</v>
@@ -2704,24 +2698,24 @@
         <v>14</v>
       </c>
       <c r="H72" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I72">
         <v>90.066999999999993</v>
       </c>
       <c r="J72" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C73" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D73" t="s">
         <v>10</v>
@@ -2739,18 +2733,18 @@
         <v>90.066999999999993</v>
       </c>
       <c r="J73" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>72</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C74" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D74" t="s">
         <v>10</v>
@@ -2762,24 +2756,24 @@
         <v>14</v>
       </c>
       <c r="H74" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I74">
         <v>90.066999999999993</v>
       </c>
       <c r="J74" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>73</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C75" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D75" t="s">
         <v>10</v>
@@ -2791,24 +2785,24 @@
         <v>12</v>
       </c>
       <c r="H75" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I75">
         <v>90.066999999999993</v>
       </c>
       <c r="J75" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>74</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C76" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D76" t="s">
         <v>10</v>
@@ -2826,18 +2820,18 @@
         <v>90.066999999999993</v>
       </c>
       <c r="J76" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>75</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C77" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D77" t="s">
         <v>10</v>
@@ -2855,18 +2849,18 @@
         <v>90.066999999999993</v>
       </c>
       <c r="J77" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>76</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C78" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D78" t="s">
         <v>10</v>
@@ -2878,24 +2872,24 @@
         <v>12</v>
       </c>
       <c r="H78" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I78">
         <v>90.066999999999993</v>
       </c>
       <c r="J78" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>77</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C79" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D79" t="s">
         <v>10</v>
@@ -2907,24 +2901,24 @@
         <v>12</v>
       </c>
       <c r="H79" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I79">
         <v>90.066999999999993</v>
       </c>
       <c r="J79" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>78</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C80" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D80" t="s">
         <v>10</v>
@@ -2936,24 +2930,24 @@
         <v>14</v>
       </c>
       <c r="H80" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I80">
         <v>90.066999999999993</v>
       </c>
       <c r="J80" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>79</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C81" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D81" t="s">
         <v>10</v>
@@ -2971,18 +2965,18 @@
         <v>90.066999999999993</v>
       </c>
       <c r="J81" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>80</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C82" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D82" t="s">
         <v>10</v>
@@ -2994,24 +2988,24 @@
         <v>14</v>
       </c>
       <c r="H82" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I82">
         <v>90.066999999999993</v>
       </c>
       <c r="J82" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>81</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C83" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D83" t="s">
         <v>10</v>
@@ -3023,24 +3017,24 @@
         <v>12</v>
       </c>
       <c r="H83" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I83">
         <v>90.066999999999993</v>
       </c>
       <c r="J83" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>82</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C84" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D84" t="s">
         <v>10</v>
@@ -3052,24 +3046,24 @@
         <v>19</v>
       </c>
       <c r="H84" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I84">
         <v>90.066999999999993</v>
       </c>
       <c r="J84" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>83</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C85" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D85" t="s">
         <v>10</v>
@@ -3087,18 +3081,18 @@
         <v>90.066999999999993</v>
       </c>
       <c r="J85" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>84</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C86" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D86" t="s">
         <v>10</v>
@@ -3116,18 +3110,18 @@
         <v>90.066999999999993</v>
       </c>
       <c r="J86" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>85</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C87" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D87" t="s">
         <v>10</v>
@@ -3145,18 +3139,18 @@
         <v>90.066999999999993</v>
       </c>
       <c r="J87" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>86</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C88" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D88" t="s">
         <v>10</v>
@@ -3168,24 +3162,24 @@
         <v>14</v>
       </c>
       <c r="H88" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I88">
         <v>90.066999999999993</v>
       </c>
       <c r="J88" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>87</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C89" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D89" t="s">
         <v>10</v>
@@ -3203,18 +3197,18 @@
         <v>90.066999999999993</v>
       </c>
       <c r="J89" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>88</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C90" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D90" t="s">
         <v>10</v>
@@ -3226,24 +3220,24 @@
         <v>19</v>
       </c>
       <c r="H90" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I90">
         <v>90.066999999999993</v>
       </c>
       <c r="J90" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>89</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C91" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D91" t="s">
         <v>10</v>
@@ -3255,24 +3249,24 @@
         <v>12</v>
       </c>
       <c r="H91" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I91">
         <v>90.066999999999993</v>
       </c>
       <c r="J91" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>90</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C92" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D92" t="s">
         <v>10</v>
@@ -3284,24 +3278,24 @@
         <v>14</v>
       </c>
       <c r="H92" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I92">
         <v>90.066999999999993</v>
       </c>
       <c r="J92" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>91</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C93" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D93" t="s">
         <v>10</v>
@@ -3319,18 +3313,18 @@
         <v>90.066999999999993</v>
       </c>
       <c r="J93" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>92</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C94" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D94" t="s">
         <v>10</v>
@@ -3348,18 +3342,18 @@
         <v>90.066999999999993</v>
       </c>
       <c r="J94" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>93</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C95" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D95" t="s">
         <v>10</v>
@@ -3371,24 +3365,24 @@
         <v>28</v>
       </c>
       <c r="H95" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I95">
-        <v>90.043000000000006</v>
+        <v>91.15</v>
       </c>
       <c r="J95" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>94</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C96" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D96" t="s">
         <v>10</v>
@@ -3397,27 +3391,27 @@
         <v>26</v>
       </c>
       <c r="F96" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H96" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I96">
-        <v>90.043000000000006</v>
+        <v>91.15</v>
       </c>
       <c r="J96" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>95</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C97" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D97" t="s">
         <v>10</v>
@@ -3429,24 +3423,24 @@
         <v>28</v>
       </c>
       <c r="H97" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I97">
-        <v>90.043000000000006</v>
+        <v>91.15</v>
       </c>
       <c r="J97" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>96</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C98" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D98" t="s">
         <v>10</v>
@@ -3455,27 +3449,27 @@
         <v>26</v>
       </c>
       <c r="F98" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H98" t="s">
         <v>13</v>
       </c>
       <c r="I98">
-        <v>90.043000000000006</v>
+        <v>91.15</v>
       </c>
       <c r="J98" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>97</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C99" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D99" t="s">
         <v>10</v>
@@ -3490,21 +3484,21 @@
         <v>15</v>
       </c>
       <c r="I99">
-        <v>90.043000000000006</v>
+        <v>91.15</v>
       </c>
       <c r="J99" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>98</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C100" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D100" t="s">
         <v>10</v>
@@ -3513,27 +3507,27 @@
         <v>26</v>
       </c>
       <c r="F100" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H100" t="s">
         <v>16</v>
       </c>
       <c r="I100">
-        <v>90.043000000000006</v>
+        <v>91.15</v>
       </c>
       <c r="J100" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>99</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C101" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D101" t="s">
         <v>10</v>
@@ -3545,24 +3539,24 @@
         <v>27</v>
       </c>
       <c r="H101" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I101">
-        <v>90.043000000000006</v>
+        <v>91.15</v>
       </c>
       <c r="J101" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>100</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C102" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D102" t="s">
         <v>10</v>
@@ -3577,21 +3571,21 @@
         <v>17</v>
       </c>
       <c r="I102">
-        <v>90.043000000000006</v>
+        <v>91.15</v>
       </c>
       <c r="J102" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>101</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C103" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D103" t="s">
         <v>10</v>
@@ -3603,24 +3597,24 @@
         <v>28</v>
       </c>
       <c r="H103" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I103">
-        <v>90.043000000000006</v>
+        <v>91.15</v>
       </c>
       <c r="J103" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>102</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C104" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D104" t="s">
         <v>10</v>
@@ -3632,24 +3626,24 @@
         <v>27</v>
       </c>
       <c r="H104" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I104">
-        <v>90.043000000000006</v>
+        <v>91.15</v>
       </c>
       <c r="J104" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>103</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C105" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D105" t="s">
         <v>10</v>
@@ -3664,21 +3658,21 @@
         <v>20</v>
       </c>
       <c r="I105">
-        <v>90.043000000000006</v>
+        <v>91.15</v>
       </c>
       <c r="J105" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="106" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>104</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C106" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D106" t="s">
         <v>10</v>
@@ -3690,24 +3684,24 @@
         <v>27</v>
       </c>
       <c r="H106" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I106">
-        <v>90.043000000000006</v>
+        <v>91.15</v>
       </c>
       <c r="J106" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="107" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>105</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C107" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D107" t="s">
         <v>10</v>
@@ -3716,16 +3710,16 @@
         <v>26</v>
       </c>
       <c r="F107" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H107" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I107">
-        <v>90.043000000000006</v>
+        <v>91.15</v>
       </c>
       <c r="J107" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
@@ -3733,7 +3727,7 @@
         <v>106</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C108" t="s">
         <v>9</v>
@@ -3748,13 +3742,13 @@
         <v>12</v>
       </c>
       <c r="H108" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I108">
         <v>87.128</v>
       </c>
       <c r="J108" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">
@@ -3762,7 +3756,7 @@
         <v>107</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C109" t="s">
         <v>9</v>
@@ -3783,7 +3777,7 @@
         <v>91.986999999999995</v>
       </c>
       <c r="J109" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
@@ -3791,7 +3785,7 @@
         <v>108</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C110" t="s">
         <v>9</v>
@@ -3812,7 +3806,7 @@
         <v>90.554000000000002</v>
       </c>
       <c r="J110" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
@@ -3820,7 +3814,7 @@
         <v>109</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C111" t="s">
         <v>9</v>
@@ -3841,7 +3835,7 @@
         <v>89.935000000000002</v>
       </c>
       <c r="J111" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
@@ -3849,7 +3843,7 @@
         <v>110</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C112" t="s">
         <v>9</v>
@@ -3870,7 +3864,7 @@
         <v>91.986999999999995</v>
       </c>
       <c r="J112" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
@@ -3878,7 +3872,7 @@
         <v>111</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C113" t="s">
         <v>9</v>
@@ -3893,13 +3887,13 @@
         <v>12</v>
       </c>
       <c r="H113" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I113">
         <v>91.986999999999995</v>
       </c>
       <c r="J113" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
@@ -3907,7 +3901,7 @@
         <v>112</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C114" t="s">
         <v>9</v>
@@ -3928,15 +3922,15 @@
         <v>90.658000000000001</v>
       </c>
       <c r="J114" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="115" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>113</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C115" t="s">
         <v>9</v>
@@ -3950,11 +3944,14 @@
       <c r="F115" t="s">
         <v>14</v>
       </c>
+      <c r="H115" t="s">
+        <v>42</v>
+      </c>
       <c r="I115">
-        <v>-100</v>
+        <v>91.986999999999995</v>
       </c>
       <c r="J115" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
@@ -3962,7 +3959,7 @@
         <v>114</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C116" t="s">
         <v>9</v>
@@ -3983,7 +3980,7 @@
         <v>91.986999999999995</v>
       </c>
       <c r="J116" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
@@ -3991,7 +3988,7 @@
         <v>115</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C117" t="s">
         <v>9</v>
@@ -4012,7 +4009,7 @@
         <v>91.986999999999995</v>
       </c>
       <c r="J117" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
@@ -4020,7 +4017,7 @@
         <v>116</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C118" t="s">
         <v>25</v>
@@ -4032,16 +4029,16 @@
         <v>26</v>
       </c>
       <c r="F118" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H118" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I118">
         <v>88.254000000000005</v>
       </c>
       <c r="J118" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
@@ -4049,7 +4046,7 @@
         <v>117</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C119" t="s">
         <v>25</v>
@@ -4061,16 +4058,16 @@
         <v>26</v>
       </c>
       <c r="F119" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H119" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I119">
         <v>88.254000000000005</v>
       </c>
       <c r="J119" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
@@ -4078,7 +4075,7 @@
         <v>118</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C120" t="s">
         <v>25</v>
@@ -4090,7 +4087,7 @@
         <v>26</v>
       </c>
       <c r="F120" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H120" t="s">
         <v>13</v>
@@ -4099,7 +4096,7 @@
         <v>88.254000000000005</v>
       </c>
       <c r="J120" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
@@ -4107,7 +4104,7 @@
         <v>119</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C121" t="s">
         <v>25</v>
@@ -4119,7 +4116,7 @@
         <v>26</v>
       </c>
       <c r="F121" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H121" t="s">
         <v>15</v>
@@ -4128,7 +4125,7 @@
         <v>87.59</v>
       </c>
       <c r="J121" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.25">
@@ -4136,7 +4133,7 @@
         <v>120</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C122" t="s">
         <v>25</v>
@@ -4157,7 +4154,7 @@
         <v>88.254000000000005</v>
       </c>
       <c r="J122" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
@@ -4165,7 +4162,7 @@
         <v>121</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C123" t="s">
         <v>25</v>
@@ -4186,7 +4183,7 @@
         <v>88.254000000000005</v>
       </c>
       <c r="J123" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.25">
@@ -4194,7 +4191,7 @@
         <v>122</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C124" t="s">
         <v>25</v>
@@ -4215,7 +4212,7 @@
         <v>88.254000000000005</v>
       </c>
       <c r="J124" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.25">
@@ -4223,7 +4220,7 @@
         <v>123</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C125" t="s">
         <v>25</v>
@@ -4238,13 +4235,13 @@
         <v>28</v>
       </c>
       <c r="H125" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I125">
         <v>88.254000000000005</v>
       </c>
       <c r="J125" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.25">
@@ -4252,7 +4249,7 @@
         <v>124</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C126" t="s">
         <v>25</v>
@@ -4267,13 +4264,13 @@
         <v>27</v>
       </c>
       <c r="H126" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I126">
         <v>88.254000000000005</v>
       </c>
       <c r="J126" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.25">
@@ -4281,7 +4278,7 @@
         <v>125</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C127" t="s">
         <v>25</v>
@@ -4302,7 +4299,7 @@
         <v>88.254000000000005</v>
       </c>
       <c r="J127" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.25">
@@ -4310,7 +4307,7 @@
         <v>126</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C128" t="s">
         <v>25</v>
@@ -4325,13 +4322,13 @@
         <v>27</v>
       </c>
       <c r="H128" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I128">
         <v>88.254000000000005</v>
       </c>
       <c r="J128" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.25">
@@ -4339,7 +4336,7 @@
         <v>127</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C129" t="s">
         <v>25</v>
@@ -4360,7 +4357,7 @@
         <v>88.254000000000005</v>
       </c>
       <c r="J129" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.25">
@@ -4368,7 +4365,7 @@
         <v>128</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C130" t="s">
         <v>25</v>
@@ -4380,16 +4377,16 @@
         <v>26</v>
       </c>
       <c r="F130" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H130" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I130">
         <v>88.254000000000005</v>
       </c>
       <c r="J130" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.25">
@@ -4397,7 +4394,7 @@
         <v>129</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C131" t="s">
         <v>25</v>
@@ -4418,7 +4415,7 @@
         <v>88.254000000000005</v>
       </c>
       <c r="J131" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.25">
@@ -4426,7 +4423,7 @@
         <v>130</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C132" t="s">
         <v>25</v>
@@ -4447,7 +4444,7 @@
         <v>88.254000000000005</v>
       </c>
       <c r="J132" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.25">
@@ -4455,7 +4452,7 @@
         <v>131</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C133" t="s">
         <v>25</v>
@@ -4476,7 +4473,7 @@
         <v>88.254000000000005</v>
       </c>
       <c r="J133" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.25">
@@ -4484,7 +4481,7 @@
         <v>132</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C134" t="s">
         <v>25</v>
@@ -4505,7 +4502,7 @@
         <v>88.254000000000005</v>
       </c>
       <c r="J134" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.25">
@@ -4513,7 +4510,7 @@
         <v>133</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C135" t="s">
         <v>25</v>
@@ -4534,7 +4531,7 @@
         <v>88.254000000000005</v>
       </c>
       <c r="J135" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.25">
@@ -4542,7 +4539,7 @@
         <v>134</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C136" t="s">
         <v>25</v>
@@ -4563,7 +4560,7 @@
         <v>88.254000000000005</v>
       </c>
       <c r="J136" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.25">
@@ -4571,7 +4568,7 @@
         <v>135</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C137" t="s">
         <v>25</v>
@@ -4586,13 +4583,13 @@
         <v>27</v>
       </c>
       <c r="H137" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I137">
         <v>88.254000000000005</v>
       </c>
       <c r="J137" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.25">
@@ -4600,7 +4597,7 @@
         <v>136</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C138" t="s">
         <v>25</v>
@@ -4621,7 +4618,7 @@
         <v>88.254000000000005</v>
       </c>
       <c r="J138" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.25">
@@ -4629,7 +4626,7 @@
         <v>137</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C139" t="s">
         <v>25</v>
@@ -4650,7 +4647,7 @@
         <v>88.254000000000005</v>
       </c>
       <c r="J139" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.25">
@@ -4658,7 +4655,7 @@
         <v>138</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C140" t="s">
         <v>9</v>
@@ -4673,13 +4670,13 @@
         <v>14</v>
       </c>
       <c r="H140" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I140">
         <v>90.658000000000001</v>
       </c>
       <c r="J140" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.25">
@@ -4687,7 +4684,7 @@
         <v>139</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C141" t="s">
         <v>9</v>
@@ -4708,7 +4705,7 @@
         <v>91.986999999999995</v>
       </c>
       <c r="J141" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.25">
@@ -4716,7 +4713,7 @@
         <v>140</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C142" t="s">
         <v>9</v>
@@ -4737,7 +4734,7 @@
         <v>90.754000000000005</v>
       </c>
       <c r="J142" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.25">
@@ -4745,7 +4742,7 @@
         <v>141</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C143" t="s">
         <v>9</v>
@@ -4766,7 +4763,7 @@
         <v>91.504999999999995</v>
       </c>
       <c r="J143" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.25">
@@ -4774,7 +4771,7 @@
         <v>142</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C144" t="s">
         <v>9</v>
@@ -4795,7 +4792,7 @@
         <v>91.986999999999995</v>
       </c>
       <c r="J144" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.25">
@@ -4803,7 +4800,7 @@
         <v>143</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C145" t="s">
         <v>9</v>
@@ -4824,7 +4821,7 @@
         <v>91.597999999999999</v>
       </c>
       <c r="J145" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.25">
@@ -4832,7 +4829,7 @@
         <v>144</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C146" t="s">
         <v>9</v>
@@ -4847,13 +4844,13 @@
         <v>14</v>
       </c>
       <c r="H146" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I146">
         <v>91.986999999999995</v>
       </c>
       <c r="J146" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.25">
@@ -4861,7 +4858,7 @@
         <v>145</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C147" t="s">
         <v>9</v>
@@ -4882,7 +4879,7 @@
         <v>91.986999999999995</v>
       </c>
       <c r="J147" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.25">
@@ -4890,7 +4887,7 @@
         <v>146</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C148" t="s">
         <v>9</v>
@@ -4911,7 +4908,7 @@
         <v>91.986999999999995</v>
       </c>
       <c r="J148" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.25">
@@ -4919,7 +4916,7 @@
         <v>147</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C149" t="s">
         <v>9</v>
@@ -4934,29 +4931,23 @@
         <v>19</v>
       </c>
       <c r="H149" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I149">
         <v>91.986999999999995</v>
       </c>
       <c r="J149" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I151">
         <f>AVERAGEIF(I2:I149, "&lt;&gt;-100")</f>
-        <v>90.016448275862075</v>
+        <v>90.300439189189149</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J149" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="9">
-      <filters>
-        <filter val="x"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:J149" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
   <headerFooter>

</xml_diff>